<commit_message>
Compatibilidad entre carpetas de Onedrive
</commit_message>
<xml_diff>
--- a/Plantilla.xlsx
+++ b/Plantilla.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rami\source\repos\Facturacion textil en Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/318745c2dd4a0186/Facturacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331807D3-9E26-49BE-B47B-293D2876C4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9DA03639-6855-48F2-BB86-1EFE8F302181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9EF1F29-C05E-4123-BC61-8A5071924405}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="4095" windowWidth="21600" windowHeight="11385" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6D90268-911F-4225-9558-77472726293D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Cantidad</t>
   </si>
@@ -61,6 +52,12 @@
   </si>
   <si>
     <t>Observaciones: archivo ""</t>
+  </si>
+  <si>
+    <t>Fecha:</t>
+  </si>
+  <si>
+    <t>Tules</t>
   </si>
 </sst>
 </file>
@@ -70,7 +67,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-2C0A]\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +107,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -281,12 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -294,9 +292,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -308,14 +303,17 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +417,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -718,42 +716,44 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G19"/>
+  <dimension ref="B1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="10.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.5546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="10"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="13"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="4" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="4" spans="2:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
@@ -773,115 +773,115 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="24"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="9"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="24"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="9"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="9"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
+    <row r="8" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
       <c r="C8" s="15"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="24"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
       <c r="C9" s="15"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="24"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="24"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="9"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="9"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="24"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="9"/>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="24"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="9"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="24"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="24"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="9"/>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="24"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="9"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G18" s="11">
@@ -889,23 +889,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+    <row r="19" spans="2:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="44" spans="4:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="D44" s="24" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="88" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;RFecha: &amp;D</oddHeader>
-    <oddFooter>&amp;C&amp;14Tules</oddFooter>
-  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>